<commit_message>
Added editorial review board for RRQ, Cascadia Organizer, & minor formatting
</commit_message>
<xml_diff>
--- a/data/courses.xlsx
+++ b/data/courses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Desktop/trial-cv/_cv_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7960634-57A6-DE44-8CF2-3A8122200FEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B80F86-2684-EF4B-99FB-3E60F8255533}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30600" yWindow="9740" windowWidth="27240" windowHeight="16440" xr2:uid="{F4143829-AF9E-244C-8EFD-6252778B5E60}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>ds</t>
   </si>
@@ -129,9 +129,6 @@
     <t>https://github.com/uo-datasci-specialization/c1-intro_data_sci</t>
   </si>
   <si>
-    <t>https://uo-datasci-specialization.github.io/c2-communicate_transform_data/</t>
-  </si>
-  <si>
     <t>https://uo-datasci-specialization.github.io/c3-fun_program_r/</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>repo</t>
   </si>
   <si>
-    <t>https://github.com/uo-datasci-specialization/c2-communicate_transform_data</t>
-  </si>
-  <si>
     <t>https://github.com/uo-datasci-specialization/c3-fun_program_r</t>
   </si>
   <si>
@@ -160,6 +154,18 @@
   </si>
   <si>
     <t>Multiple regression in educational research [supervised teaching]</t>
+  </si>
+  <si>
+    <t>2019/2020</t>
+  </si>
+  <si>
+    <t>https://uo-datasci-specialization.github.io/c2-dataviz-2020/</t>
+  </si>
+  <si>
+    <t>https://github.com/uo-datasci-specialization/c2-dataviz-2020</t>
+  </si>
+  <si>
+    <t>27553/27120</t>
   </si>
 </sst>
 </file>
@@ -514,7 +520,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,10 +548,10 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
         <v>38</v>
-      </c>
-      <c r="I1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -584,11 +590,11 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3">
-        <v>2019</v>
-      </c>
-      <c r="E3">
-        <v>27553</v>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -597,10 +603,10 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -626,10 +632,10 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -655,7 +661,7 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -681,7 +687,7 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -707,7 +713,7 @@
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -776,7 +782,7 @@
         <v>28</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -816,7 +822,7 @@
         <v>2015</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G12">
         <v>4</v>

</xml_diff>

<commit_message>
changes since last update - prior to promotion file (if I apply)
</commit_message>
<xml_diff>
--- a/data/courses.xlsx
+++ b/data/courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B80F86-2684-EF4B-99FB-3E60F8255533}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A42CC2-016D-2548-80E9-D7C1E7D00569}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30600" yWindow="9740" windowWidth="27240" windowHeight="16440" xr2:uid="{F4143829-AF9E-244C-8EFD-6252778B5E60}"/>
+    <workbookView xWindow="21800" yWindow="7120" windowWidth="27240" windowHeight="16440" xr2:uid="{F4143829-AF9E-244C-8EFD-6252778B5E60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>ds</t>
   </si>
@@ -45,24 +45,9 @@
     <t>title</t>
   </si>
   <si>
-    <t>Introduction to data science with R</t>
-  </si>
-  <si>
-    <t>Communicating and transforming data</t>
-  </si>
-  <si>
-    <t>Functional programming with R</t>
-  </si>
-  <si>
-    <t>Applied predictive modeling</t>
-  </si>
-  <si>
     <t>Capstone</t>
   </si>
   <si>
-    <t>[planned]</t>
-  </si>
-  <si>
     <t>Multiple regression in educational research</t>
   </si>
   <si>
@@ -129,12 +114,6 @@
     <t>https://github.com/uo-datasci-specialization/c1-intro_data_sci</t>
   </si>
   <si>
-    <t>https://uo-datasci-specialization.github.io/c3-fun_program_r/</t>
-  </si>
-  <si>
-    <t>https://www.datalorax.com/vita/mr/mr/</t>
-  </si>
-  <si>
     <t>https://github.com/datalorax/CourseR</t>
   </si>
   <si>
@@ -144,21 +123,9 @@
     <t>repo</t>
   </si>
   <si>
-    <t>https://github.com/uo-datasci-specialization/c3-fun_program_r</t>
-  </si>
-  <si>
-    <t>https://github.com/uo-datasci-specialization/c4-pred_modeling</t>
-  </si>
-  <si>
-    <t>https://github.com/uo-datasci-specialization/c5-capstone</t>
-  </si>
-  <si>
     <t>Multiple regression in educational research [supervised teaching]</t>
   </si>
   <si>
-    <t>2019/2020</t>
-  </si>
-  <si>
     <t>https://uo-datasci-specialization.github.io/c2-dataviz-2020/</t>
   </si>
   <si>
@@ -166,19 +133,78 @@
   </si>
   <si>
     <t>27553/27120</t>
+  </si>
+  <si>
+    <t>2019/2020/2021 [planned]</t>
+  </si>
+  <si>
+    <t>EDLD 651: Introduction to Educational Data Science (EDS)</t>
+  </si>
+  <si>
+    <t>EDLD 652: Data visualization for EDS</t>
+  </si>
+  <si>
+    <t>EDLD 653: Functional programming for EDS</t>
+  </si>
+  <si>
+    <t>EDLD 654: Machine learning for EDS</t>
+  </si>
+  <si>
+    <t>2021 [planned]</t>
+  </si>
+  <si>
+    <t>spring</t>
+  </si>
+  <si>
+    <t>Hierarchical Linear Modeling II</t>
+  </si>
+  <si>
+    <t>https://uo-datasci-specialization.github.io/c4-ml-fall-2020/</t>
+  </si>
+  <si>
+    <t>https://uo-datasci-specialization.github.io/c3-fun_program2020/</t>
+  </si>
+  <si>
+    <t>https://github.com/uo-datasci-specialization/c3-fun_program2020</t>
+  </si>
+  <si>
+    <t>https://github.com/uo-datasci-specialization/c4-ml-fall-2020</t>
+  </si>
+  <si>
+    <t>35699/32066</t>
+  </si>
+  <si>
+    <t>37108/16924</t>
+  </si>
+  <si>
+    <t>https://github.com/datalorax/mr-fall18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -198,13 +224,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -517,20 +547,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80AB2D6-D787-8D4A-BD11-32CAE09CA316}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -545,13 +580,13 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -562,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>2018</v>
@@ -571,13 +606,13 @@
         <v>12074</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="G2">
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -588,25 +623,25 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
-        <v>44</v>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -617,25 +652,25 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>2019</v>
-      </c>
-      <c r="E4">
-        <v>35699</v>
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -646,22 +681,25 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>2020</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
+      <c r="E5" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -672,22 +710,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6">
-        <v>2020</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G6">
         <v>4</v>
-      </c>
-      <c r="I6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -698,22 +730,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7">
-        <v>2018</v>
-      </c>
-      <c r="E7">
-        <v>17258</v>
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -724,19 +750,22 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>2018</v>
       </c>
       <c r="E8">
-        <v>40797</v>
+        <v>17258</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G8">
         <v>3</v>
+      </c>
+      <c r="I8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -747,82 +776,85 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D9">
-        <v>2017</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
+        <v>2018</v>
+      </c>
+      <c r="E9">
+        <v>40797</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>2017</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" t="s">
-        <v>36</v>
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
         <v>22</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11">
-        <v>2017</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>23</v>
       </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
+      <c r="I11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>2015</v>
+        <v>2017</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="G12">
         <v>4</v>
@@ -830,19 +862,42 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>2015</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" t="s">
-        <v>30</v>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{434FBEC4-E05E-3140-82B3-28805D027D95}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add aera 21 conf and AERA Open in-press article
</commit_message>
<xml_diff>
--- a/data/courses.xlsx
+++ b/data/courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/anderson-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A42CC2-016D-2548-80E9-D7C1E7D00569}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AE7442-4753-2C47-B10B-D3C667DBDEB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21800" yWindow="7120" windowWidth="27240" windowHeight="16440" xr2:uid="{F4143829-AF9E-244C-8EFD-6252778B5E60}"/>
+    <workbookView xWindow="37320" yWindow="1620" windowWidth="27240" windowHeight="16440" xr2:uid="{F4143829-AF9E-244C-8EFD-6252778B5E60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>ds</t>
   </si>
@@ -126,18 +126,6 @@
     <t>Multiple regression in educational research [supervised teaching]</t>
   </si>
   <si>
-    <t>https://uo-datasci-specialization.github.io/c2-dataviz-2020/</t>
-  </si>
-  <si>
-    <t>https://github.com/uo-datasci-specialization/c2-dataviz-2020</t>
-  </si>
-  <si>
-    <t>27553/27120</t>
-  </si>
-  <si>
-    <t>2019/2020/2021 [planned]</t>
-  </si>
-  <si>
     <t>EDLD 651: Introduction to Educational Data Science (EDS)</t>
   </si>
   <si>
@@ -150,34 +138,49 @@
     <t>EDLD 654: Machine learning for EDS</t>
   </si>
   <si>
-    <t>2021 [planned]</t>
-  </si>
-  <si>
-    <t>spring</t>
-  </si>
-  <si>
     <t>Hierarchical Linear Modeling II</t>
   </si>
   <si>
     <t>https://uo-datasci-specialization.github.io/c4-ml-fall-2020/</t>
   </si>
   <si>
-    <t>https://uo-datasci-specialization.github.io/c3-fun_program2020/</t>
-  </si>
-  <si>
-    <t>https://github.com/uo-datasci-specialization/c3-fun_program2020</t>
-  </si>
-  <si>
     <t>https://github.com/uo-datasci-specialization/c4-ml-fall-2020</t>
   </si>
   <si>
-    <t>35699/32066</t>
-  </si>
-  <si>
     <t>37108/16924</t>
   </si>
   <si>
     <t>https://github.com/datalorax/mr-fall18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019/2020/2021 </t>
+  </si>
+  <si>
+    <t>2019/2020/2021</t>
+  </si>
+  <si>
+    <t>https://dataviz-2021.netlify.app/</t>
+  </si>
+  <si>
+    <t>https://github.com/uo-datasci-specialization/c2-dataviz-2021</t>
+  </si>
+  <si>
+    <t>https://fp-2021.netlify.app/</t>
+  </si>
+  <si>
+    <t>https://github.com/uo-datasci-specialization/c3-fp-2021</t>
+  </si>
+  <si>
+    <t>https://mlm2-2021.netlify.app/</t>
+  </si>
+  <si>
+    <t>https://github.com/datalorax/mlm2</t>
+  </si>
+  <si>
+    <t>35699/32066/36713</t>
+  </si>
+  <si>
+    <t>27553/27120/27056</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,7 +609,7 @@
         <v>12074</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -626,22 +629,22 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -655,22 +658,22 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -687,19 +690,19 @@
         <v>2020</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -712,8 +715,11 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>41</v>
+      <c r="D6">
+        <v>2021</v>
+      </c>
+      <c r="E6">
+        <v>27140</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
@@ -730,16 +736,25 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>2021</v>
+      </c>
+      <c r="E7">
+        <v>36724</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G7">
         <v>3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -765,7 +780,7 @@
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -895,9 +910,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{434FBEC4-E05E-3140-82B3-28805D027D95}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>